<commit_message>
update : bird, object pool
- 세 프리팹 레이어 설정
- BirdData : 점수, 스폰확률 추가
- 오브젝트 풀링 : 종마다 큐 생성
</commit_message>
<xml_diff>
--- a/Assets/Resources/DataFiles/BirdData.xlsx
+++ b/Assets/Resources/DataFiles/BirdData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bluejoy\Documents\GitHub\VR_birdwatching\Assets\Resources\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AA30D8-1319-4375-A448-F98ECD60EEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3B686E-332B-4EFA-81B8-27EB2A87476B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Crow</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -46,14 +46,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>청둥오리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mallard</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>검독수리</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -102,10 +94,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>청둥오리 서식지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>검독수리 서식지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -130,10 +118,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>청둥오리 개체수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>검독수리 개체수</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -158,10 +142,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>청둥오리 특징</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>검독수리 특징</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -179,6 +159,14 @@
   </si>
   <si>
     <t>멕시코양지니 특징</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>누적 확률</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>점수</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -536,10 +524,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -550,7 +538,7 @@
     <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -558,132 +546,157 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>39</v>
+      <c r="G7">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix : dictionary error
</commit_message>
<xml_diff>
--- a/Assets/Resources/DataFiles/BirdData.xlsx
+++ b/Assets/Resources/DataFiles/BirdData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bluejoy\Documents\GitHub\VR_birdwatching\Assets\Resources\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3B686E-332B-4EFA-81B8-27EB2A87476B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F20FD9F-8FC7-441A-B550-778412401AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Crow</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -62,111 +62,95 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>멕시코양지니</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>북미갈매기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국수리부엉이</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국까마귀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>서식지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>개체수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>특징</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>미국까마귀 서식지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>검독수리 서식지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국수리부엉이 서식지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>집비둘기 서식지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>북미갈매기 서식지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>멕시코양지니 서식지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국까마귀 개체수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>검독수리 개체수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국수리부엉이 개체수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>집비둘기 개체수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>북미갈매기 개체수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>멕시코양지니 개체수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국까마귀 특징</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>검독수리 특징</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국수리부엉이 특징</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>집비둘기 특징</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>북미갈매기 특징</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>멕시코양지니 특징</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>누적 확률</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>점수</t>
+    <t>확률</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>포인트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유라시아, 북아메리카, 일부 아프리카 지역</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>관심 필요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>까마귀</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 없음.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성체 기준 몸 길이는 48~52cm이며, 무게는 약 300~600g으로 대게 수컷이 암컷보다 크다. 매우 지능적이며 인간 환경에 적응할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>수리부엉이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유라시아 대부분 지역, 유럽 전 지역</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체적으로 어두운 갈색을 띄며, 머리와 목에 더 연한 깃털이 있다. 익장이 2m에 달하며 최대 시속 240km로 비행할 수 있다. 먹이는 주로 토끼, 다람쥐, 청설모, 거북, 뱀 등이 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">키는 위아래로 60 ~ 75cm, 익장 131 ~ 188cm. 매우 튼튼한 다리, 날카로운 발톱을 가지고 있다. 몸에 있는 부드러운 솜털이 소리를 흡수하기 때문에 거의 무소음에 가까운 비행이 가능하다. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전세계</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1년 내내 번식이 가능하다. 최고 시속 112km를 자랑하며 기억력이 높고, 인간의 얼굴을 구별할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대한민국 멸종위기 I급.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>갈매기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닷가에 주로 서식하며 그 외에도 습지, 내륙의 호수 등에서도 흔히 볼 수 있다. 몸길이는 약 40cm이고 날개를 폈을 때는 120cm 정도이다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다양한 계통으로 종이 나뉘어져 있으며 잡식성으로 곡식 낟알이나 벌레를 잡아먹는다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닷가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>참새</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전세계에 걸쳐 분포. 종마다 상이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>멸종 위기 등급</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -527,15 +511,15 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="17.875" customWidth="1"/>
-    <col min="3" max="3" width="22.125" customWidth="1"/>
-    <col min="4" max="4" width="22.375" customWidth="1"/>
-    <col min="5" max="5" width="58" customWidth="1"/>
+    <col min="3" max="3" width="48.625" customWidth="1"/>
+    <col min="4" max="4" width="41.125" customWidth="1"/>
+    <col min="5" max="5" width="78.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -546,19 +530,19 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
@@ -566,16 +550,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -592,13 +576,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F3">
         <v>30</v>
@@ -612,16 +596,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F4">
         <v>50</v>
@@ -638,13 +622,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -658,16 +642,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -681,16 +665,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="F7">
         <v>3</v>

</xml_diff>